<commit_message>
add excel parser and test data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Adtech/PG/Repos/Selenium/data_driven_simple/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C42603F-531C-D14D-A674-1F14BD861282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C413D0-E600-B640-A940-772C3AE2F6D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
+    <workbookView xWindow="43120" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +22,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Florin</t>
+  </si>
+  <si>
+    <t>Barbu</t>
+  </si>
+  <si>
+    <t>Andra</t>
+  </si>
+  <si>
+    <t>Barbu-Corfariu</t>
+  </si>
+  <si>
+    <t>123dsfsd</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,12 +400,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109C616F-C422-4643-966C-111CC93709FE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E18:E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>500123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new test + some changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Adtech/PG/Repos/Selenium/data_driven_simple/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E97EFDD-6389-A240-B95A-C258C19224F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE47F456-18E7-C34E-BD27-F5DE79DCCE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43340" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
+    <workbookView xWindow="43340" yWindow="1780" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>firstname</t>
   </si>
@@ -55,6 +56,18 @@
   </si>
   <si>
     <t>500123b</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Florin Barbu</t>
+  </si>
+  <si>
+    <t>EURO</t>
   </si>
 </sst>
 </file>
@@ -408,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109C616F-C422-4643-966C-111CC93709FE}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,4 +475,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B924F502-3F9A-DD45-BBBF-C3FDC37222EC}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add stepts for test 3
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Adtech/PG/Repos/Selenium/data_driven_simple/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE47F456-18E7-C34E-BD27-F5DE79DCCE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CEC0A3-5113-C54B-B6C8-97257CD5FD60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43340" yWindow="1780" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>firstname</t>
   </si>
@@ -67,7 +67,10 @@
     <t>Florin Barbu</t>
   </si>
   <si>
-    <t>EURO</t>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>Account created successfully with account Number</t>
   </si>
 </sst>
 </file>
@@ -479,29 +482,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B924F502-3F9A-DD45-BBBF-C3FDC37222EC}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add functionality for test skip
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Adtech/PG/Repos/Selenium/data_driven_simple/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CEC0A3-5113-C54B-B6C8-97257CD5FD60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0276661D-7645-B743-BDF5-A9FC7CE86938}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43340" yWindow="1780" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
+    <workbookView xWindow="5780" yWindow="1460" windowWidth="28040" windowHeight="17440" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>firstname</t>
   </si>
@@ -71,6 +72,27 @@
   </si>
   <si>
     <t>Account created successfully with account Number</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>loginAsBankManagerTest</t>
+  </si>
+  <si>
+    <t>addCustomerTest</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>openAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -421,6 +443,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C25DEA6-BA35-7042-9340-BB97C5800BD6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109C616F-C422-4643-966C-111CC93709FE}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -480,11 +552,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B924F502-3F9A-DD45-BBBF-C3FDC37222EC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
use hashtable for data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Adtech/PG/Repos/Selenium/data_driven_simple/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0276661D-7645-B743-BDF5-A9FC7CE86938}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E24022-0CA4-DC43-8184-C5D13C8DA54D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="1460" windowWidth="28040" windowHeight="17440" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
+    <workbookView xWindow="5780" yWindow="1460" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{24CA32E3-BAF9-1342-B925-ABD2516A54E2}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -27,16 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Florin</t>
   </si>
@@ -44,9 +35,6 @@
     <t>Barbu</t>
   </si>
   <si>
-    <t>alerttext</t>
-  </si>
-  <si>
     <t>Customer added successfully</t>
   </si>
   <si>
@@ -93,6 +81,33 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Coto</t>
+  </si>
+  <si>
+    <t>Vladimir</t>
+  </si>
+  <si>
+    <t>MOS</t>
+  </si>
+  <si>
+    <t>CRACIUN</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postCode</t>
+  </si>
+  <si>
+    <t>alertText</t>
+  </si>
+  <si>
+    <t>runMode</t>
   </si>
 </sst>
 </file>
@@ -446,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C25DEA6-BA35-7042-9340-BB97C5800BD6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -457,34 +472,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -494,57 +509,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109C616F-C422-4643-966C-111CC93709FE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>500123</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>123123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>666</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -556,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B924F502-3F9A-DD45-BBBF-C3FDC37222EC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,24 +627,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>